<commit_message>
sucesso, na parte de acgar redes independentes e aleatorias
</commit_message>
<xml_diff>
--- a/fuction_ensemble_1/redes-ensemble-s/mse_sup/1000_model_10_8_23.xlsx
+++ b/fuction_ensemble_1/redes-ensemble-s/mse_sup/1000_model_10_8_23.xlsx
@@ -480,7 +480,7 @@
         <v>3.299645433692669</v>
       </c>
       <c r="D3" t="n">
-        <v>3.13437819480896</v>
+        <v>3.134378433227539</v>
       </c>
     </row>
     <row r="4">
@@ -550,7 +550,7 @@
         <v>1.790142199564391</v>
       </c>
       <c r="D8" t="n">
-        <v>1.923522591590881</v>
+        <v>1.92352283000946</v>
       </c>
     </row>
     <row r="9">
@@ -592,7 +592,7 @@
         <v>1.404551743365336</v>
       </c>
       <c r="D11" t="n">
-        <v>1.273473381996155</v>
+        <v>1.273473143577576</v>
       </c>
     </row>
     <row r="12">
@@ -620,7 +620,7 @@
         <v>1.385995091465572</v>
       </c>
       <c r="D13" t="n">
-        <v>1.012737989425659</v>
+        <v>1.012738227844238</v>
       </c>
     </row>
     <row r="14">
@@ -634,7 +634,7 @@
         <v>1.430324041922637</v>
       </c>
       <c r="D14" t="n">
-        <v>0.9811383485794067</v>
+        <v>0.9811382293701172</v>
       </c>
     </row>
     <row r="15">
@@ -662,7 +662,7 @@
         <v>1.598267225469177</v>
       </c>
       <c r="D16" t="n">
-        <v>1.237718462944031</v>
+        <v>1.23771858215332</v>
       </c>
     </row>
     <row r="17">
@@ -676,7 +676,7 @@
         <v>1.712503714724715</v>
       </c>
       <c r="D17" t="n">
-        <v>1.538273692131042</v>
+        <v>1.538273453712463</v>
       </c>
     </row>
     <row r="18">
@@ -690,7 +690,7 @@
         <v>1.841427758198229</v>
       </c>
       <c r="D18" t="n">
-        <v>1.896246910095215</v>
+        <v>1.896247148513794</v>
       </c>
     </row>
     <row r="19">
@@ -914,7 +914,7 @@
         <v>3.173507168895993</v>
       </c>
       <c r="D34" t="n">
-        <v>3.362977981567383</v>
+        <v>3.362977743148804</v>
       </c>
     </row>
     <row r="35">
@@ -928,7 +928,7 @@
         <v>2.944953424467837</v>
       </c>
       <c r="D35" t="n">
-        <v>3.163558006286621</v>
+        <v>3.1635582447052</v>
       </c>
     </row>
     <row r="36">
@@ -1054,7 +1054,7 @@
         <v>1.020666773095332</v>
       </c>
       <c r="D44" t="n">
-        <v>1.111146807670593</v>
+        <v>1.111147046089172</v>
       </c>
     </row>
     <row r="45">
@@ -1068,7 +1068,7 @@
         <v>1.031303082240741</v>
       </c>
       <c r="D45" t="n">
-        <v>1.00059986114502</v>
+        <v>1.000599980354309</v>
       </c>
     </row>
     <row r="46">
@@ -1082,7 +1082,7 @@
         <v>1.075632032697805</v>
       </c>
       <c r="D46" t="n">
-        <v>0.9641146659851074</v>
+        <v>0.9641149044036865</v>
       </c>
     </row>
     <row r="47">
@@ -1096,7 +1096,7 @@
         <v>1.148046603653651</v>
       </c>
       <c r="D47" t="n">
-        <v>1.028694033622742</v>
+        <v>1.028694152832031</v>
       </c>
     </row>
     <row r="48">
@@ -1124,7 +1124,7 @@
         <v>1.357811705499883</v>
       </c>
       <c r="D49" t="n">
-        <v>1.513842344284058</v>
+        <v>1.513842582702637</v>
       </c>
     </row>
     <row r="50">
@@ -1152,7 +1152,7 @@
         <v>1.626475781118616</v>
       </c>
       <c r="D51" t="n">
-        <v>2.201207160949707</v>
+        <v>2.201206922531128</v>
       </c>
     </row>
     <row r="52">
@@ -1376,7 +1376,7 @@
         <v>2.75413347852185</v>
       </c>
       <c r="D67" t="n">
-        <v>3.195508241653442</v>
+        <v>3.195508480072021</v>
       </c>
     </row>
     <row r="68">
@@ -1390,7 +1390,7 @@
         <v>2.442311014711867</v>
       </c>
       <c r="D68" t="n">
-        <v>2.973987817764282</v>
+        <v>2.973988056182861</v>
       </c>
     </row>
     <row r="69">
@@ -1502,7 +1502,7 @@
         <v>0.8298468271493438</v>
       </c>
       <c r="D76" t="n">
-        <v>1.105567216873169</v>
+        <v>1.105567097663879</v>
       </c>
     </row>
     <row r="77">
@@ -1530,7 +1530,7 @@
         <v>0.8848120867518172</v>
       </c>
       <c r="D78" t="n">
-        <v>0.9479273557662964</v>
+        <v>0.9479274749755859</v>
       </c>
     </row>
     <row r="79">
@@ -1810,7 +1810,7 @@
         <v>2.919828224085738</v>
       </c>
       <c r="D98" t="n">
-        <v>3.430683135986328</v>
+        <v>3.430683374404907</v>
       </c>
     </row>
     <row r="99">
@@ -1894,7 +1894,7 @@
         <v>1.181771245529304</v>
       </c>
       <c r="D104" t="n">
-        <v>1.984365820884705</v>
+        <v>1.984365701675415</v>
       </c>
     </row>
     <row r="105">
@@ -1908,7 +1908,7 @@
         <v>0.9987009572345125</v>
       </c>
       <c r="D105" t="n">
-        <v>1.729145169258118</v>
+        <v>1.729145050048828</v>
       </c>
     </row>
     <row r="106">
@@ -2202,7 +2202,7 @@
         <v>2.272194692149099</v>
       </c>
       <c r="D126" t="n">
-        <v>2.446853876113892</v>
+        <v>2.446854114532471</v>
       </c>
     </row>
     <row r="127">
@@ -2328,7 +2328,7 @@
         <v>1.45570207604664</v>
       </c>
       <c r="D135" t="n">
-        <v>2.279318809509277</v>
+        <v>2.279318571090698</v>
       </c>
     </row>
     <row r="136">
@@ -2342,7 +2342,7 @@
         <v>1.216233490586281</v>
       </c>
       <c r="D136" t="n">
-        <v>2.01045036315918</v>
+        <v>2.010450124740601</v>
       </c>
     </row>
     <row r="137">
@@ -2356,7 +2356,7 @@
         <v>1.03316320229149</v>
       </c>
       <c r="D137" t="n">
-        <v>1.748874425888062</v>
+        <v>1.748874306678772</v>
       </c>
     </row>
     <row r="138">
@@ -2384,7 +2384,7 @@
         <v>0.8306430343872264</v>
       </c>
       <c r="D139" t="n">
-        <v>1.283098936080933</v>
+        <v>1.283098697662354</v>
       </c>
     </row>
     <row r="140">
@@ -2426,7 +2426,7 @@
         <v>0.8564153329445274</v>
       </c>
       <c r="D142" t="n">
-        <v>0.9224866628646851</v>
+        <v>0.922486424446106</v>
       </c>
     </row>
     <row r="143">
@@ -2482,7 +2482,7 @@
         <v>1.267519049220119</v>
       </c>
       <c r="D146" t="n">
-        <v>1.810147166252136</v>
+        <v>1.810146927833557</v>
       </c>
     </row>
     <row r="147">
@@ -2510,7 +2510,7 @@
         <v>1.553840270544643</v>
       </c>
       <c r="D148" t="n">
-        <v>2.379950523376465</v>
+        <v>2.379950284957886</v>
       </c>
     </row>
     <row r="149">
@@ -2580,7 +2580,7 @@
         <v>2.220854016399727</v>
       </c>
       <c r="D153" t="n">
-        <v>2.573899745941162</v>
+        <v>2.573899984359741</v>
       </c>
     </row>
     <row r="154">
@@ -2706,7 +2706,7 @@
         <v>3.060649487226699</v>
       </c>
       <c r="D162" t="n">
-        <v>3.524622201919556</v>
+        <v>3.524622440338135</v>
       </c>
     </row>
     <row r="163">
@@ -2818,7 +2818,7 @@
         <v>1.012325463520111</v>
       </c>
       <c r="D170" t="n">
-        <v>1.520973801612854</v>
+        <v>1.520974040031433</v>
       </c>
     </row>
     <row r="171">
@@ -3322,7 +3322,7 @@
         <v>1.119794265593114</v>
       </c>
       <c r="D206" t="n">
-        <v>0.9173291921615601</v>
+        <v>0.9173290729522705</v>
       </c>
     </row>
     <row r="207">
@@ -3350,7 +3350,7 @@
         <v>1.287737449139653</v>
       </c>
       <c r="D208" t="n">
-        <v>1.149223446846008</v>
+        <v>1.149223208427429</v>
       </c>
     </row>
     <row r="209">
@@ -3630,7 +3630,7 @@
         <v>2.866494599745228</v>
       </c>
       <c r="D228" t="n">
-        <v>3.22880220413208</v>
+        <v>3.228801965713501</v>
       </c>
     </row>
     <row r="229">
@@ -4134,7 +4134,7 @@
         <v>1.873020991472165</v>
       </c>
       <c r="D264" t="n">
-        <v>2.195805549621582</v>
+        <v>2.195805788040161</v>
       </c>
     </row>
     <row r="265">
@@ -4232,7 +4232,7 @@
         <v>1.585617404786256</v>
       </c>
       <c r="D271" t="n">
-        <v>0.9992058277130127</v>
+        <v>0.9992060661315918</v>
       </c>
     </row>
     <row r="272">
@@ -4288,7 +4288,7 @@
         <v>2.064046582251221</v>
       </c>
       <c r="D275" t="n">
-        <v>2.152572154998779</v>
+        <v>2.1525719165802</v>
       </c>
     </row>
     <row r="276">
@@ -4400,7 +4400,7 @@
         <v>3.00890445405681</v>
       </c>
       <c r="D283" t="n">
-        <v>2.549230098724365</v>
+        <v>2.549230337142944</v>
       </c>
     </row>
     <row r="284">
@@ -4512,7 +4512,7 @@
         <v>3.584666542510784</v>
       </c>
       <c r="D291" t="n">
-        <v>3.658821105957031</v>
+        <v>3.65882134437561</v>
       </c>
     </row>
     <row r="292">
@@ -4526,7 +4526,7 @@
         <v>3.272844078700802</v>
       </c>
       <c r="D292" t="n">
-        <v>3.420209884643555</v>
+        <v>3.420210123062134</v>
       </c>
     </row>
     <row r="293">
@@ -4540,7 +4540,7 @@
         <v>2.933126623944096</v>
       </c>
       <c r="D293" t="n">
-        <v>3.157393217086792</v>
+        <v>3.157393455505371</v>
       </c>
     </row>
     <row r="294">
@@ -4666,7 +4666,7 @@
         <v>1.715345150740752</v>
       </c>
       <c r="D302" t="n">
-        <v>0.9907361268997192</v>
+        <v>0.9907362461090088</v>
       </c>
     </row>
     <row r="303">
@@ -4736,7 +4736,7 @@
         <v>2.266188899161562</v>
       </c>
       <c r="D307" t="n">
-        <v>2.187654733657837</v>
+        <v>2.187654495239258</v>
       </c>
     </row>
     <row r="308">
@@ -4750,7 +4750,7 @@
         <v>2.412770088340868</v>
       </c>
       <c r="D308" t="n">
-        <v>2.424912691116333</v>
+        <v>2.424912929534912</v>
       </c>
     </row>
     <row r="309">
@@ -4988,7 +4988,7 @@
         <v>3.11551355621029</v>
       </c>
       <c r="D325" t="n">
-        <v>3.272914886474609</v>
+        <v>3.272915124893188</v>
       </c>
     </row>
     <row r="326">
@@ -5058,7 +5058,7 @@
         <v>1.947283195498546</v>
       </c>
       <c r="D330" t="n">
-        <v>1.771254658699036</v>
+        <v>1.771254897117615</v>
       </c>
     </row>
     <row r="331">
@@ -5072,7 +5072,7 @@
         <v>1.871959784449645</v>
       </c>
       <c r="D331" t="n">
-        <v>1.505372762680054</v>
+        <v>1.505373001098633</v>
       </c>
     </row>
     <row r="332">
@@ -5114,7 +5114,7 @@
         <v>1.897732083006946</v>
       </c>
       <c r="D334" t="n">
-        <v>1.047445178031921</v>
+        <v>1.0474454164505</v>
       </c>
     </row>
     <row r="335">
@@ -5142,7 +5142,7 @@
         <v>2.065675266553486</v>
       </c>
       <c r="D336" t="n">
-        <v>1.270886063575745</v>
+        <v>1.270885825157166</v>
       </c>
     </row>
     <row r="337">
@@ -5394,7 +5394,7 @@
         <v>4.139868088781944</v>
       </c>
       <c r="D354" t="n">
-        <v>4.138069152832031</v>
+        <v>4.138068675994873</v>
       </c>
     </row>
     <row r="355">
@@ -5408,7 +5408,7 @@
         <v>3.911314344353789</v>
       </c>
       <c r="D355" t="n">
-        <v>3.918602228164673</v>
+        <v>3.918601989746094</v>
       </c>
     </row>
     <row r="356">
@@ -5464,7 +5464,7 @@
         <v>2.641279695685869</v>
       </c>
       <c r="D359" t="n">
-        <v>2.796255588531494</v>
+        <v>2.796255826950073</v>
       </c>
     </row>
     <row r="360">
@@ -5548,7 +5548,7 @@
         <v>1.997664002126692</v>
       </c>
       <c r="D365" t="n">
-        <v>1.197132349014282</v>
+        <v>1.197131991386414</v>
       </c>
     </row>
     <row r="366">
@@ -5618,7 +5618,7 @@
         <v>2.453096668859348</v>
       </c>
       <c r="D370" t="n">
-        <v>1.990778207778931</v>
+        <v>1.99077832698822</v>
       </c>
     </row>
     <row r="371">
@@ -5646,7 +5646,7 @@
         <v>2.739417890183872</v>
       </c>
       <c r="D372" t="n">
-        <v>2.542288303375244</v>
+        <v>2.542288541793823</v>
       </c>
     </row>
     <row r="373">
@@ -5870,7 +5870,7 @@
         <v>3.687340798017104</v>
       </c>
       <c r="D388" t="n">
-        <v>3.800872564315796</v>
+        <v>3.800872802734375</v>
       </c>
     </row>
     <row r="389">
@@ -5912,7 +5912,7 @@
         <v>2.729128613159167</v>
       </c>
       <c r="D391" t="n">
-        <v>2.913594007492065</v>
+        <v>2.913594245910645</v>
       </c>
     </row>
     <row r="392">
@@ -5926,7 +5926,7 @@
         <v>2.489660027698808</v>
       </c>
       <c r="D392" t="n">
-        <v>2.591461896896362</v>
+        <v>2.591461658477783</v>
       </c>
     </row>
     <row r="393">
@@ -5940,7 +5940,7 @@
         <v>2.306589739404017</v>
       </c>
       <c r="D393" t="n">
-        <v>2.271587610244751</v>
+        <v>2.27158784866333</v>
       </c>
     </row>
     <row r="394">
@@ -5968,7 +5968,7 @@
         <v>2.104069571499753</v>
       </c>
       <c r="D395" t="n">
-        <v>1.687626123428345</v>
+        <v>1.687626361846924</v>
       </c>
     </row>
     <row r="396">
@@ -6038,7 +6038,7 @@
         <v>2.297785053603594</v>
       </c>
       <c r="D400" t="n">
-        <v>1.42952823638916</v>
+        <v>1.42952835559845</v>
       </c>
     </row>
     <row r="401">
@@ -6094,7 +6094,7 @@
         <v>2.82726680765717</v>
       </c>
       <c r="D404" t="n">
-        <v>2.62407112121582</v>
+        <v>2.624071359634399</v>
       </c>
     </row>
     <row r="405">
@@ -6318,7 +6318,7 @@
         <v>3.702259259979531</v>
       </c>
       <c r="D420" t="n">
-        <v>3.902604579925537</v>
+        <v>3.902604818344116</v>
       </c>
     </row>
     <row r="421">
@@ -6332,7 +6332,7 @@
         <v>3.362541805222826</v>
       </c>
       <c r="D421" t="n">
-        <v>3.626587629318237</v>
+        <v>3.626587867736816</v>
       </c>
     </row>
     <row r="422">
@@ -6388,7 +6388,7 @@
         <v>2.321508201366445</v>
       </c>
       <c r="D425" t="n">
-        <v>2.36299204826355</v>
+        <v>2.362992286682129</v>
       </c>
     </row>
     <row r="426">
@@ -7228,7 +7228,7 @@
         <v>3.132319382194215</v>
       </c>
       <c r="D485" t="n">
-        <v>3.574212312698364</v>
+        <v>3.574212074279785</v>
       </c>
     </row>
     <row r="486">
@@ -7382,7 +7382,7 @@
         <v>2.082481092537411</v>
       </c>
       <c r="D496" t="n">
-        <v>1.557576775550842</v>
+        <v>1.557576656341553</v>
       </c>
     </row>
     <row r="497">
@@ -7396,7 +7396,7 @@
         <v>2.196717581792949</v>
       </c>
       <c r="D497" t="n">
-        <v>1.869553685188293</v>
+        <v>1.869553804397583</v>
       </c>
     </row>
     <row r="498">
@@ -7690,7 +7690,7 @@
         <v>2.560649187714273</v>
       </c>
       <c r="D518" t="n">
-        <v>3.03556227684021</v>
+        <v>3.035562515258789</v>
       </c>
     </row>
     <row r="519">
@@ -7732,7 +7732,7 @@
         <v>1.847505236767772</v>
       </c>
       <c r="D521" t="n">
-        <v>2.113687038421631</v>
+        <v>2.11368727684021</v>
       </c>
     </row>
     <row r="522">
@@ -7746,7 +7746,7 @@
         <v>1.72030847991241</v>
       </c>
       <c r="D522" t="n">
-        <v>1.818520069122314</v>
+        <v>1.818520307540894</v>
       </c>
     </row>
     <row r="523">
@@ -7900,7 +7900,7 @@
         <v>2.517297892375212</v>
       </c>
       <c r="D533" t="n">
-        <v>2.815203428268433</v>
+        <v>2.815203189849854</v>
       </c>
     </row>
     <row r="534">
@@ -8068,7 +8068,7 @@
         <v>2.900401593987162</v>
       </c>
       <c r="D545" t="n">
-        <v>2.732969045639038</v>
+        <v>2.732969284057617</v>
       </c>
     </row>
     <row r="546">
@@ -8110,7 +8110,7 @@
         <v>2.919942780411361</v>
       </c>
       <c r="D548" t="n">
-        <v>3.191879272460938</v>
+        <v>3.191879510879517</v>
       </c>
     </row>
     <row r="549">
@@ -8180,7 +8180,7 @@
         <v>1.539191721798274</v>
       </c>
       <c r="D553" t="n">
-        <v>1.745912432670593</v>
+        <v>1.745912075042725</v>
       </c>
     </row>
     <row r="554">
@@ -8208,7 +8208,7 @@
         <v>1.33667155389401</v>
       </c>
       <c r="D555" t="n">
-        <v>1.196630239486694</v>
+        <v>1.196630358695984</v>
       </c>
     </row>
     <row r="556">
@@ -8222,7 +8222,7 @@
         <v>1.307478592848837</v>
       </c>
       <c r="D556" t="n">
-        <v>0.9846348762512207</v>
+        <v>0.9846346378326416</v>
       </c>
     </row>
     <row r="557">
@@ -8264,7 +8264,7 @@
         <v>1.434858423407156</v>
       </c>
       <c r="D559" t="n">
-        <v>0.877996563911438</v>
+        <v>0.8779968023300171</v>
       </c>
     </row>
     <row r="560">
@@ -8292,7 +8292,7 @@
         <v>1.644623525253389</v>
       </c>
       <c r="D561" t="n">
-        <v>1.431973695755005</v>
+        <v>1.431973457336426</v>
       </c>
     </row>
     <row r="562">
@@ -8334,7 +8334,7 @@
         <v>2.059868790051427</v>
       </c>
       <c r="D564" t="n">
-        <v>2.397011995315552</v>
+        <v>2.397011756896973</v>
       </c>
     </row>
     <row r="565">
@@ -8404,7 +8404,7 @@
         <v>2.726882535906511</v>
       </c>
       <c r="D569" t="n">
-        <v>2.673527002334595</v>
+        <v>2.673526763916016</v>
       </c>
     </row>
     <row r="570">
@@ -8474,7 +8474,7 @@
         <v>2.812685456712861</v>
       </c>
       <c r="D574" t="n">
-        <v>2.603410243988037</v>
+        <v>2.603410005569458</v>
       </c>
     </row>
     <row r="575">
@@ -8614,7 +8614,7 @@
         <v>1.382350718960405</v>
       </c>
       <c r="D584" t="n">
-        <v>1.66488254070282</v>
+        <v>1.664882659912109</v>
       </c>
     </row>
     <row r="585">
@@ -8740,7 +8740,7 @@
         <v>1.304712234120729</v>
       </c>
       <c r="D593" t="n">
-        <v>1.057413458824158</v>
+        <v>1.057413220405579</v>
       </c>
     </row>
     <row r="594">
@@ -8866,7 +8866,7 @@
         <v>2.46772775263487</v>
       </c>
       <c r="D602" t="n">
-        <v>2.317581653594971</v>
+        <v>2.31758189201355</v>
       </c>
     </row>
     <row r="603">
@@ -8894,7 +8894,7 @@
         <v>2.535453672077408</v>
       </c>
       <c r="D604" t="n">
-        <v>2.298507452011108</v>
+        <v>2.298507213592529</v>
       </c>
     </row>
     <row r="605">
@@ -9020,7 +9020,7 @@
         <v>1.912954058486604</v>
       </c>
       <c r="D613" t="n">
-        <v>2.310011625289917</v>
+        <v>2.310011386871338</v>
       </c>
     </row>
     <row r="614">
@@ -9160,7 +9160,7 @@
         <v>0.767587156239105</v>
       </c>
       <c r="D623" t="n">
-        <v>0.1905921697616577</v>
+        <v>0.1905925273895264</v>
       </c>
     </row>
     <row r="624">
@@ -9202,7 +9202,7 @@
         <v>1.106276301558852</v>
       </c>
       <c r="D626" t="n">
-        <v>1.12557327747345</v>
+        <v>1.125572919845581</v>
       </c>
     </row>
     <row r="627">
@@ -9216,7 +9216,7 @@
         <v>1.24601633370407</v>
       </c>
       <c r="D627" t="n">
-        <v>1.460841298103333</v>
+        <v>1.460841655731201</v>
       </c>
     </row>
     <row r="628">
@@ -9300,7 +9300,7 @@
         <v>2.05961126873846</v>
       </c>
       <c r="D633" t="n">
-        <v>1.984429478645325</v>
+        <v>1.984429240226746</v>
       </c>
     </row>
     <row r="634">
@@ -9412,7 +9412,7 @@
         <v>1.924816811849612</v>
       </c>
       <c r="D641" t="n">
-        <v>1.910101532936096</v>
+        <v>1.910101294517517</v>
       </c>
     </row>
     <row r="642">
@@ -9510,7 +9510,7 @@
         <v>0.7893197318704457</v>
       </c>
       <c r="D648" t="n">
-        <v>1.255110621452332</v>
+        <v>1.255110859870911</v>
       </c>
     </row>
     <row r="649">
@@ -9580,7 +9580,7 @@
         <v>0.3851726237716271</v>
       </c>
       <c r="D653" t="n">
-        <v>-0.005654936190694571</v>
+        <v>-0.005654459353536367</v>
       </c>
     </row>
     <row r="654">
@@ -9594,7 +9594,7 @@
         <v>0.4295015742286916</v>
       </c>
       <c r="D654" t="n">
-        <v>-0.05461180582642555</v>
+        <v>-0.05461156740784645</v>
       </c>
     </row>
     <row r="655">
@@ -9636,7 +9636,7 @@
         <v>0.7116812470307694</v>
       </c>
       <c r="D657" t="n">
-        <v>0.5755983591079712</v>
+        <v>0.5755985975265503</v>
       </c>
     </row>
     <row r="658">
@@ -9748,7 +9748,7 @@
         <v>1.793940257683891</v>
       </c>
       <c r="D665" t="n">
-        <v>1.764000415802002</v>
+        <v>1.764000535011292</v>
       </c>
     </row>
     <row r="666">
@@ -9776,7 +9776,7 @@
         <v>1.925203194455091</v>
       </c>
       <c r="D667" t="n">
-        <v>1.733918190002441</v>
+        <v>1.733917951583862</v>
       </c>
     </row>
     <row r="668">
@@ -9790,7 +9790,7 @@
         <v>1.942422684987449</v>
       </c>
       <c r="D668" t="n">
-        <v>1.717408657073975</v>
+        <v>1.717408776283264</v>
       </c>
     </row>
     <row r="669">
@@ -9846,7 +9846,7 @@
         <v>1.73228790275219</v>
       </c>
       <c r="D672" t="n">
-        <v>1.659972310066223</v>
+        <v>1.659972667694092</v>
       </c>
     </row>
     <row r="673">
@@ -9888,7 +9888,7 @@
         <v>2.13919895140194</v>
       </c>
       <c r="D675" t="n">
-        <v>2.68898344039917</v>
+        <v>2.688983678817749</v>
       </c>
     </row>
     <row r="676">
@@ -9986,7 +9986,7 @@
         <v>0.319428672123508</v>
       </c>
       <c r="D682" t="n">
-        <v>0.5866507291793823</v>
+        <v>0.5866506099700928</v>
       </c>
     </row>
     <row r="683">
@@ -10000,7 +10000,7 @@
         <v>0.2441052610746066</v>
       </c>
       <c r="D683" t="n">
-        <v>0.3138788938522339</v>
+        <v>0.3138785362243652</v>
       </c>
     </row>
     <row r="684">
@@ -10028,7 +10028,7 @@
         <v>0.2255486091748435</v>
       </c>
       <c r="D685" t="n">
-        <v>-0.06004965677857399</v>
+        <v>-0.06004941835999489</v>
       </c>
     </row>
     <row r="686">
@@ -10182,7 +10182,7 @@
         <v>1.528175019310493</v>
       </c>
       <c r="D696" t="n">
-        <v>1.680789113044739</v>
+        <v>1.680789351463318</v>
       </c>
     </row>
     <row r="697">
@@ -10238,7 +10238,7 @@
         <v>1.782798670390665</v>
       </c>
       <c r="D700" t="n">
-        <v>1.611835837364197</v>
+        <v>1.611835598945618</v>
       </c>
     </row>
     <row r="701">
@@ -10294,7 +10294,7 @@
         <v>1.572663888155407</v>
       </c>
       <c r="D704" t="n">
-        <v>1.537937521934509</v>
+        <v>1.537937760353088</v>
       </c>
     </row>
     <row r="705">
@@ -10336,7 +10336,7 @@
         <v>2.113445173984622</v>
       </c>
       <c r="D707" t="n">
-        <v>2.701101779937744</v>
+        <v>2.701101541519165</v>
       </c>
     </row>
     <row r="708">
@@ -10350,7 +10350,7 @@
         <v>1.801622710174639</v>
       </c>
       <c r="D708" t="n">
-        <v>2.443469047546387</v>
+        <v>2.443468809127808</v>
       </c>
     </row>
     <row r="709">
@@ -10364,7 +10364,7 @@
         <v>1.461905255417934</v>
       </c>
       <c r="D709" t="n">
-        <v>2.161665439605713</v>
+        <v>2.161665678024292</v>
       </c>
     </row>
     <row r="710">
@@ -10462,7 +10462,7 @@
         <v>0.1891585226121162</v>
       </c>
       <c r="D716" t="n">
-        <v>0.09569143503904343</v>
+        <v>0.09569191187620163</v>
       </c>
     </row>
     <row r="717">
@@ -10504,7 +10504,7 @@
         <v>0.3165383531704351</v>
       </c>
       <c r="D719" t="n">
-        <v>-0.02733052335679531</v>
+        <v>-0.02733004651963711</v>
       </c>
     </row>
     <row r="720">
@@ -10518,7 +10518,7 @@
         <v>0.4120669657611298</v>
       </c>
       <c r="D720" t="n">
-        <v>0.1911245584487915</v>
+        <v>0.1911238431930542</v>
       </c>
     </row>
     <row r="721">
@@ -10532,7 +10532,7 @@
         <v>0.5263034550166679</v>
       </c>
       <c r="D721" t="n">
-        <v>0.5204174518585205</v>
+        <v>0.5204175710678101</v>
       </c>
     </row>
     <row r="722">
@@ -10546,7 +10546,7 @@
         <v>0.655227498490182</v>
       </c>
       <c r="D722" t="n">
-        <v>0.8864356279373169</v>
+        <v>0.8864352703094482</v>
       </c>
     </row>
     <row r="723">
@@ -10574,7 +10574,7 @@
         <v>0.9415487198147059</v>
       </c>
       <c r="D724" t="n">
-        <v>1.43584406375885</v>
+        <v>1.435844302177429</v>
       </c>
     </row>
     <row r="725">
@@ -10602,7 +10602,7 @@
         <v>1.237508583695971</v>
       </c>
       <c r="D726" t="n">
-        <v>1.641843914985657</v>
+        <v>1.641844153404236</v>
       </c>
     </row>
     <row r="727">
@@ -10686,7 +10686,7 @@
         <v>1.757044892973348</v>
       </c>
       <c r="D732" t="n">
-        <v>1.591961622238159</v>
+        <v>1.591961860656738</v>
       </c>
     </row>
     <row r="733">
@@ -10700,7 +10700,7 @@
         <v>1.740737894775215</v>
       </c>
       <c r="D733" t="n">
-        <v>1.570735692977905</v>
+        <v>1.570735335350037</v>
       </c>
     </row>
     <row r="734">
@@ -10826,7 +10826,7 @@
         <v>1.24274650183506</v>
       </c>
       <c r="D742" t="n">
-        <v>1.887838959693909</v>
+        <v>1.887839078903198</v>
       </c>
     </row>
     <row r="743">
@@ -10896,7 +10896,7 @@
         <v>0.327082382984295</v>
       </c>
       <c r="D747" t="n">
-        <v>0.3523871898651123</v>
+        <v>0.3523876667022705</v>
       </c>
     </row>
     <row r="748">
@@ -10994,7 +10994,7 @@
         <v>0.763958397817188</v>
       </c>
       <c r="D754" t="n">
-        <v>0.920317530632019</v>
+        <v>0.9203177690505981</v>
       </c>
     </row>
     <row r="755">
@@ -11036,7 +11036,7 @@
         <v>1.199395206495999</v>
       </c>
       <c r="D757" t="n">
-        <v>1.598719000816345</v>
+        <v>1.598719239234924</v>
       </c>
     </row>
     <row r="758">
@@ -11078,7 +11078,7 @@
         <v>1.611152141220181</v>
       </c>
       <c r="D760" t="n">
-        <v>1.688240170478821</v>
+        <v>1.6882404088974</v>
       </c>
     </row>
     <row r="761">
@@ -11176,7 +11176,7 @@
         <v>1.7344351995571</v>
       </c>
       <c r="D767" t="n">
-        <v>1.551673650741577</v>
+        <v>1.551673889160156</v>
       </c>
     </row>
     <row r="768">
@@ -11274,7 +11274,7 @@
         <v>1.453892733539852</v>
       </c>
       <c r="D774" t="n">
-        <v>1.926404476165771</v>
+        <v>1.926404237747192</v>
       </c>
     </row>
     <row r="775">
@@ -11316,7 +11316,7 @@
         <v>0.7407487825933514</v>
       </c>
       <c r="D777" t="n">
-        <v>0.973167896270752</v>
+        <v>0.9731676578521729</v>
       </c>
     </row>
     <row r="778">
@@ -11358,7 +11358,7 @@
         <v>0.5090356536439153</v>
       </c>
       <c r="D780" t="n">
-        <v>0.1764844655990601</v>
+        <v>0.1764849424362183</v>
       </c>
     </row>
     <row r="781">
@@ -11428,7 +11428,7 @@
         <v>0.8461805860484668</v>
       </c>
       <c r="D785" t="n">
-        <v>0.6053440570831299</v>
+        <v>0.6053435802459717</v>
       </c>
     </row>
     <row r="786">
@@ -11498,7 +11498,7 @@
         <v>1.55738571472777</v>
       </c>
       <c r="D790" t="n">
-        <v>1.702278137207031</v>
+        <v>1.70227837562561</v>
       </c>
     </row>
     <row r="791">
@@ -11680,7 +11680,7 @@
         <v>2.685768998120597</v>
       </c>
       <c r="D803" t="n">
-        <v>2.803121328353882</v>
+        <v>2.803121089935303</v>
       </c>
     </row>
     <row r="804">
@@ -11708,7 +11708,7 @@
         <v>2.034229079553909</v>
       </c>
       <c r="D805" t="n">
-        <v>2.267330169677734</v>
+        <v>2.267329931259155</v>
       </c>
     </row>
     <row r="806">
@@ -11820,7 +11820,7 @@
         <v>0.7721186558935005</v>
       </c>
       <c r="D813" t="n">
-        <v>0.08191274851560593</v>
+        <v>0.08191322535276413</v>
       </c>
     </row>
     <row r="814">
@@ -11918,7 +11918,7 @@
         <v>1.513872543950681</v>
       </c>
       <c r="D820" t="n">
-        <v>1.551320433616638</v>
+        <v>1.551320672035217</v>
       </c>
     </row>
     <row r="821">
@@ -11932,7 +11932,7 @@
         <v>1.662988131304967</v>
       </c>
       <c r="D821" t="n">
-        <v>1.680712699890137</v>
+        <v>1.680712461471558</v>
       </c>
     </row>
     <row r="822">
@@ -11974,7 +11974,7 @@
         <v>2.07474506602915</v>
       </c>
       <c r="D824" t="n">
-        <v>1.76215934753418</v>
+        <v>1.762159585952759</v>
       </c>
     </row>
     <row r="825">
@@ -12044,7 +12044,7 @@
         <v>2.31306171891119</v>
       </c>
       <c r="D829" t="n">
-        <v>1.666519641876221</v>
+        <v>1.666519403457642</v>
       </c>
     </row>
     <row r="830">
@@ -12128,7 +12128,7 @@
         <v>2.903916735691156</v>
       </c>
       <c r="D835" t="n">
-        <v>2.838726997375488</v>
+        <v>2.838726758956909</v>
       </c>
     </row>
     <row r="836">
@@ -12310,7 +12310,7 @@
         <v>1.202538527467664</v>
       </c>
       <c r="D848" t="n">
-        <v>0.3947153091430664</v>
+        <v>0.3947149515151978</v>
       </c>
     </row>
     <row r="849">
@@ -12366,7 +12366,7 @@
         <v>1.73202028152124</v>
       </c>
       <c r="D852" t="n">
-        <v>1.600194215774536</v>
+        <v>1.600193977355957</v>
       </c>
     </row>
     <row r="853">
@@ -12450,7 +12450,7 @@
         <v>2.479790535237343</v>
       </c>
       <c r="D858" t="n">
-        <v>1.766533732414246</v>
+        <v>1.766533851623535</v>
       </c>
     </row>
     <row r="859">
@@ -12492,7 +12492,7 @@
         <v>2.53120945648175</v>
       </c>
       <c r="D861" t="n">
-        <v>1.703721880912781</v>
+        <v>1.70372211933136</v>
       </c>
     </row>
     <row r="862">
@@ -12506,7 +12506,7 @@
         <v>2.484836948182673</v>
       </c>
       <c r="D862" t="n">
-        <v>1.684582233428955</v>
+        <v>1.684582471847534</v>
       </c>
     </row>
     <row r="863">
@@ -12534,7 +12534,7 @@
         <v>2.337381672444623</v>
       </c>
       <c r="D864" t="n">
-        <v>1.649581789970398</v>
+        <v>1.649581551551819</v>
       </c>
     </row>
     <row r="865">
@@ -12632,7 +12632,7 @@
         <v>1.750921522997698</v>
       </c>
       <c r="D871" t="n">
-        <v>1.759304523468018</v>
+        <v>1.759304881095886</v>
       </c>
     </row>
     <row r="872">
@@ -12758,7 +12758,7 @@
         <v>1.319577963442125</v>
       </c>
       <c r="D880" t="n">
-        <v>0.4601670503616333</v>
+        <v>0.460167407989502</v>
       </c>
     </row>
     <row r="881">
@@ -12772,7 +12772,7 @@
         <v>1.433814452697663</v>
       </c>
       <c r="D881" t="n">
-        <v>0.7847648859024048</v>
+        <v>0.7847651243209839</v>
       </c>
     </row>
     <row r="882">
@@ -12800,7 +12800,7 @@
         <v>1.702478528316396</v>
       </c>
       <c r="D883" t="n">
-        <v>1.440675258636475</v>
+        <v>1.440674781799316</v>
       </c>
     </row>
     <row r="884">
@@ -12828,7 +12828,7 @@
         <v>1.998175304849988</v>
       </c>
       <c r="D885" t="n">
-        <v>1.773246884346008</v>
+        <v>1.773246645927429</v>
       </c>
     </row>
     <row r="886">
@@ -12870,7 +12870,7 @@
         <v>2.40993223957417</v>
       </c>
       <c r="D888" t="n">
-        <v>1.841091871261597</v>
+        <v>1.841092109680176</v>
       </c>
     </row>
     <row r="889">
@@ -12912,7 +12912,7 @@
         <v>2.647336400121985</v>
       </c>
       <c r="D891" t="n">
-        <v>1.781226396560669</v>
+        <v>1.78122615814209</v>
       </c>
     </row>
     <row r="892">
@@ -13080,7 +13080,7 @@
         <v>1.733760527841484</v>
       </c>
       <c r="D903" t="n">
-        <v>1.811845779418945</v>
+        <v>1.811845898628235</v>
       </c>
     </row>
     <row r="904">
@@ -13094,7 +13094,7 @@
         <v>1.494291942381125</v>
       </c>
       <c r="D904" t="n">
-        <v>1.507949948310852</v>
+        <v>1.507949709892273</v>
       </c>
     </row>
     <row r="905">
@@ -13122,7 +13122,7 @@
         <v>1.184024897230971</v>
       </c>
       <c r="D906" t="n">
-        <v>0.9132853746414185</v>
+        <v>0.9132858514785767</v>
       </c>
     </row>
     <row r="907">
@@ -13164,7 +13164,7 @@
         <v>1.090144834282307</v>
       </c>
       <c r="D909" t="n">
-        <v>0.2799522876739502</v>
+        <v>0.2799526453018188</v>
       </c>
     </row>
     <row r="910">
@@ -13220,7 +13220,7 @@
         <v>1.416653457541449</v>
       </c>
       <c r="D913" t="n">
-        <v>0.8522670269012451</v>
+        <v>0.8522672653198242</v>
       </c>
     </row>
     <row r="914">
@@ -13234,7 +13234,7 @@
         <v>1.545577501014963</v>
       </c>
       <c r="D914" t="n">
-        <v>1.202046513557434</v>
+        <v>1.202046632766724</v>
       </c>
     </row>
     <row r="915">
@@ -13248,7 +13248,7 @@
         <v>1.685317533160181</v>
       </c>
       <c r="D915" t="n">
-        <v>1.499529957771301</v>
+        <v>1.499529838562012</v>
       </c>
     </row>
     <row r="916">
@@ -13262,7 +13262,7 @@
         <v>1.831898722339487</v>
       </c>
       <c r="D916" t="n">
-        <v>1.705183863639832</v>
+        <v>1.705183625221252</v>
       </c>
     </row>
     <row r="917">
@@ -13276,7 +13276,7 @@
         <v>1.981014309693773</v>
       </c>
       <c r="D917" t="n">
-        <v>1.822718739509583</v>
+        <v>1.822718620300293</v>
       </c>
     </row>
     <row r="918">
@@ -13318,7 +13318,7 @@
         <v>2.392771244417956</v>
       </c>
       <c r="D920" t="n">
-        <v>1.881623148918152</v>
+        <v>1.881622910499573</v>
       </c>
     </row>
     <row r="921">
@@ -13388,7 +13388,7 @@
         <v>2.631087897299996</v>
       </c>
       <c r="D925" t="n">
-        <v>1.772249698638916</v>
+        <v>1.772249937057495</v>
       </c>
     </row>
     <row r="926">
@@ -13430,7 +13430,7 @@
         <v>2.43726011326287</v>
       </c>
       <c r="D928" t="n">
-        <v>1.716033697128296</v>
+        <v>1.716033935546875</v>
       </c>
     </row>
     <row r="929">
@@ -13500,7 +13500,7 @@
         <v>2.217592180867846</v>
       </c>
       <c r="D933" t="n">
-        <v>2.428770542144775</v>
+        <v>2.428770780563354</v>
       </c>
     </row>
     <row r="934">
@@ -13528,7 +13528,7 @@
         <v>1.599097450766615</v>
       </c>
       <c r="D935" t="n">
-        <v>1.86439061164856</v>
+        <v>1.864390850067139</v>
       </c>
     </row>
     <row r="936">
@@ -13542,7 +13542,7 @@
         <v>1.359628865306256</v>
       </c>
       <c r="D936" t="n">
-        <v>1.567013263702393</v>
+        <v>1.567013382911682</v>
       </c>
     </row>
     <row r="937">
@@ -13626,7 +13626,7 @@
         <v>0.9998107076645018</v>
       </c>
       <c r="D942" t="n">
-        <v>0.3056488037109375</v>
+        <v>0.3056483268737793</v>
       </c>
     </row>
     <row r="943">
@@ -13696,7 +13696,7 @@
         <v>1.550654456085312</v>
       </c>
       <c r="D947" t="n">
-        <v>1.561984181404114</v>
+        <v>1.561984658241272</v>
       </c>
     </row>
     <row r="948">
@@ -13710,7 +13710,7 @@
         <v>1.697235645264618</v>
       </c>
       <c r="D948" t="n">
-        <v>1.762398958206177</v>
+        <v>1.762399077415466</v>
       </c>
     </row>
     <row r="949">
@@ -13724,7 +13724,7 @@
         <v>1.846351232618904</v>
       </c>
       <c r="D949" t="n">
-        <v>1.875245213508606</v>
+        <v>1.875245451927185</v>
       </c>
     </row>
     <row r="950">
@@ -13738,7 +13738,7 @@
         <v>1.993195509145883</v>
       </c>
       <c r="D950" t="n">
-        <v>1.924582719802856</v>
+        <v>1.924582958221436</v>
       </c>
     </row>
     <row r="951">
@@ -13752,7 +13752,7 @@
         <v>2.13239900052997</v>
       </c>
       <c r="D951" t="n">
-        <v>1.934926271438599</v>
+        <v>1.93492603302002</v>
       </c>
     </row>
     <row r="952">
@@ -13822,7 +13822,7 @@
         <v>2.512731818423259</v>
       </c>
       <c r="D956" t="n">
-        <v>1.828548073768616</v>
+        <v>1.828548431396484</v>
       </c>
     </row>
     <row r="957">
@@ -13836,7 +13836,7 @@
         <v>2.496424820225128</v>
       </c>
       <c r="D957" t="n">
-        <v>1.805577993392944</v>
+        <v>1.805577874183655</v>
       </c>
     </row>
     <row r="958">
@@ -13878,7 +13878,7 @@
         <v>2.302597036188001</v>
       </c>
       <c r="D960" t="n">
-        <v>1.746377348899841</v>
+        <v>1.74637758731842</v>
       </c>
     </row>
     <row r="961">
@@ -14046,7 +14046,7 @@
         <v>0.7565508702861141</v>
       </c>
       <c r="D972" t="n">
-        <v>0.5782260894775391</v>
+        <v>0.5782256126403809</v>
       </c>
     </row>
     <row r="973">
@@ -14088,7 +14088,7 @@
         <v>0.8839307008444326</v>
       </c>
       <c r="D975" t="n">
-        <v>0.4637807607650757</v>
+        <v>0.4637811183929443</v>
       </c>
     </row>
     <row r="976">
@@ -14158,7 +14158,7 @@
         <v>1.508941067488704</v>
       </c>
       <c r="D980" t="n">
-        <v>1.823358774185181</v>
+        <v>1.82335889339447</v>
       </c>
     </row>
     <row r="981">
@@ -14186,7 +14186,7 @@
         <v>1.804900931369969</v>
       </c>
       <c r="D982" t="n">
-        <v>1.976568818092346</v>
+        <v>1.976569056510925</v>
       </c>
     </row>
     <row r="983">
@@ -14200,7 +14200,7 @@
         <v>1.944104422754056</v>
       </c>
       <c r="D983" t="n">
-        <v>1.98336923122406</v>
+        <v>1.983369469642639</v>
       </c>
     </row>
     <row r="984">
@@ -14242,7 +14242,7 @@
         <v>2.256711321204807</v>
       </c>
       <c r="D986" t="n">
-        <v>1.918682932853699</v>
+        <v>1.918683171272278</v>
       </c>
     </row>
     <row r="987">
@@ -14312,7 +14312,7 @@
         <v>2.193096647904091</v>
       </c>
       <c r="D991" t="n">
-        <v>1.79600977897644</v>
+        <v>1.796009659767151</v>
       </c>
     </row>
     <row r="992">
@@ -14326,7 +14326,7 @@
         <v>2.114302458412086</v>
       </c>
       <c r="D992" t="n">
-        <v>1.776554584503174</v>
+        <v>1.776554942131042</v>
       </c>
     </row>
     <row r="993">
@@ -14340,7 +14340,7 @@
         <v>2.04116035645494</v>
       </c>
       <c r="D993" t="n">
-        <v>1.758525729179382</v>
+        <v>1.758525490760803</v>
       </c>
     </row>
     <row r="994">
@@ -14396,7 +14396,7 @@
         <v>1.873697198389866</v>
       </c>
       <c r="D997" t="n">
-        <v>2.496809482574463</v>
+        <v>2.496809005737305</v>
       </c>
     </row>
     <row r="998">
@@ -14452,7 +14452,7 @@
         <v>0.8326635945334839</v>
       </c>
       <c r="D1001" t="n">
-        <v>1.399013519287109</v>
+        <v>1.399013876914978</v>
       </c>
     </row>
     <row r="1002">
@@ -14494,7 +14494,7 @@
         <v>0.6009504655840479</v>
       </c>
       <c r="D1004" t="n">
-        <v>0.6553080081939697</v>
+        <v>0.6553083658218384</v>
       </c>
     </row>
     <row r="1005">
@@ -14522,7 +14522,7 @@
         <v>0.6559157251865215</v>
       </c>
       <c r="D1006" t="n">
-        <v>0.4634802341461182</v>
+        <v>0.4634807109832764</v>
       </c>
     </row>
     <row r="1007">
@@ -14536,7 +14536,7 @@
         <v>0.7283302961423663</v>
       </c>
       <c r="D1007" t="n">
-        <v>0.5445146560668945</v>
+        <v>0.5445141792297363</v>
       </c>
     </row>
     <row r="1008">
@@ -14564,7 +14564,7 @@
         <v>0.9380953979885993</v>
       </c>
       <c r="D1009" t="n">
-        <v>1.077804327011108</v>
+        <v>1.077804803848267</v>
       </c>
     </row>
     <row r="1010">
@@ -14592,7 +14592,7 @@
         <v>1.206759473607332</v>
       </c>
       <c r="D1011" t="n">
-        <v>1.698274731636047</v>
+        <v>1.698274970054626</v>
       </c>
     </row>
     <row r="1012">
@@ -14606,7 +14606,7 @@
         <v>1.353340662786637</v>
       </c>
       <c r="D1012" t="n">
-        <v>1.888132810592651</v>
+        <v>1.888132572174072</v>
       </c>
     </row>
     <row r="1013">
@@ -14676,7 +14676,7 @@
         <v>2.020354408641721</v>
       </c>
       <c r="D1017" t="n">
-        <v>1.991880774497986</v>
+        <v>1.991880655288696</v>
       </c>
     </row>
     <row r="1018">
@@ -14718,7 +14718,7 @@
         <v>2.168836835945279</v>
       </c>
       <c r="D1020" t="n">
-        <v>1.90324878692627</v>
+        <v>1.903249025344849</v>
       </c>
     </row>
     <row r="1021">
@@ -14774,7 +14774,7 @@
         <v>1.95870205371002</v>
       </c>
       <c r="D1024" t="n">
-        <v>1.807790637016296</v>
+        <v>1.807790398597717</v>
       </c>
     </row>
     <row r="1025">

</xml_diff>